<commit_message>
check lists for new fields
</commit_message>
<xml_diff>
--- a/check-list.xlsx
+++ b/check-list.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT_NEW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT_NEW\git\check-lists_bag-reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA08419-9FD6-475D-9F79-49A3DFD39E60}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4337B255-442B-45DB-8C5B-B748FCE14E90}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{EB6332A4-5CD7-43C2-AA75-05F29A5AC152}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" activeTab="3" xr2:uid="{EB6332A4-5CD7-43C2-AA75-05F29A5AC152}"/>
   </bookViews>
   <sheets>
     <sheet name="field &quot;name&quot;" sheetId="1" r:id="rId1"/>
     <sheet name="field &quot;surname&quot;" sheetId="2" r:id="rId2"/>
+    <sheet name="field &quot;email&quot;" sheetId="3" r:id="rId3"/>
+    <sheet name="field &quot;password&quot;" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="160">
   <si>
     <t>ID</t>
   </si>
@@ -59,9 +61,6 @@
   </si>
   <si>
     <t xml:space="preserve">                                                                                                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                           Testing of field "name"</t>
   </si>
   <si>
     <r>
@@ -202,12 +201,383 @@
   <si>
     <t>Enter "Valer.iya", another fields are filled due to specification</t>
   </si>
+  <si>
+    <t>Filling the field "surname" with valid data type</t>
+  </si>
+  <si>
+    <t>Filling the field "surname" with min. allowed number of letetrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling the field "surname" with one letter less than min. allowed </t>
+  </si>
+  <si>
+    <t>Filling the field "surname" with one letter more than min. allowed</t>
+  </si>
+  <si>
+    <t>Filling the field "surname" with max. allowed number of letetrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling the field "surname" with one letter less than max. allowed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling the field "surname" with Cyrillic </t>
+  </si>
+  <si>
+    <t>Filling the field "surname" with uppercase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAILED </t>
+  </si>
+  <si>
+    <t>Enter "Stryapan", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>Enter "St", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "S", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Filling the field "name" with one letter more than max. allowed</t>
+  </si>
+  <si>
+    <t>Enter 256 Latin letters, another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Filling the field "surname" with one letter more than max. allowed</t>
+  </si>
+  <si>
+    <t>Enter "Стряпан", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "STRYAPAN", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter " Stryapan", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "Stryapan ", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "Stryap-an", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "Stryap'an", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "Strya-pa'n",  another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "Stryapan@", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "(Stryapan)", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "Stryapan$", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "Stryapan#", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "Stryap.an", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling the field "email" with Cyrillic </t>
+  </si>
+  <si>
+    <t>Enter "лера@gmail.com", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling the field "email" without at </t>
+  </si>
+  <si>
+    <t>Enter "leragmail.com", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don’t fill the field "email" </t>
+  </si>
+  <si>
+    <t>Enter "#lera@gmail.com", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling the field "email" with min. allowed number of letetrs before an at </t>
+  </si>
+  <si>
+    <t>Enter "le@gmail.com", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "ler@gmail.com", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "l@gmail.com", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling the field "email" with one letter more than min. allowed  before an at </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling the field "email" with one letter less than min. allowed  before an at </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Filling the field "email" with max. allowed  number of letetrs before an at </t>
+  </si>
+  <si>
+    <t>Enter 128 Latin letters before an at, another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling the field "email" with one letter more than max. allowed  before an at </t>
+  </si>
+  <si>
+    <t>Filling the field "email" with one letter less than max. allowed  before an at</t>
+  </si>
+  <si>
+    <t>Enter 129 Latin letters before an at, another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter 127 Latin letters before an at, another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Filling the field "email" with space before an at</t>
+  </si>
+  <si>
+    <t>Enter "lera @gmail.com", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Filling the field "email" with nubmers after an at</t>
+  </si>
+  <si>
+    <t>Enter "lera@00gmail.com", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             Testing of field "name" according to the documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    Testing of field "surname" according to the documentation</t>
+  </si>
+  <si>
+    <t>Filling the field "email" with a special character as the first symbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling the field "email" with underscore before an at </t>
+  </si>
+  <si>
+    <t>Enter "le_ra@gmail.com", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling the field "email" with dot before an at </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling the field "email" with dash before an at </t>
+  </si>
+  <si>
+    <t>Enter "le.ra@gmail.com", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "le-ra@gmail.com", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling the field "email" with two ats </t>
+  </si>
+  <si>
+    <t>Enter "lera@@gmail.com", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Filling the field "email" with max. allowed number of letetrs in second-level domain</t>
+  </si>
+  <si>
+    <t>Filling the field "email" with one letter less than max. allowed in second-level domain</t>
+  </si>
+  <si>
+    <t>Filling the field "email" with one letter more than max. allowed in second-level domain</t>
+  </si>
+  <si>
+    <t>Filling the field "email" with min. allowed number of letetrs in second-level domain</t>
+  </si>
+  <si>
+    <t>Filling the field "email" with one letter less than min. allowed in second-level domain</t>
+  </si>
+  <si>
+    <t>Filling the field "email" with one letter more than min. allowed in second-level domain</t>
+  </si>
+  <si>
+    <t>Enter 17 Latin letters in second-level domain, another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter 1 Latin letters in second-level domain, another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter 16 Latin letters in second-level domain, another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter 15 Latin letters in second-level domain, another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter 2 Latin letters in second-level domain, another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter 3 Latin letters in second-level domain, another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Filling the field "password" with min. allowed number of letetrs</t>
+  </si>
+  <si>
+    <t>Filling the field "password" with one letter less than min. allowed</t>
+  </si>
+  <si>
+    <t>Filling the field "password" with one letter more than min. allowed</t>
+  </si>
+  <si>
+    <t>Filling the field "password" with max. allowed number of letetrs</t>
+  </si>
+  <si>
+    <t>Filling the field "password" with one letter less than max. allowed</t>
+  </si>
+  <si>
+    <t>Filling the field "password" with one letter more than max. allowed</t>
+  </si>
+  <si>
+    <t>Enter 32 Latin letters (particularly min. 1 special character, min. 1 number, min. 1 uppercase letter) another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter 31 Latin letters (particularly min. 1 special character, min. 1 number, min. 1 uppercase letter), another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter 33 Latin letters (particularly min. 1 special character, min. 1 number, min. 1 uppercase letter), another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling the field "password" with a space </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Filling the field "password" without 1 special character</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Filling the field "password" without 1 number</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Filling the field "password" without 1 uppercase letter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don’t fill the field "password" </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Check list for ITCareer's website registration form </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">                                             Testing of field "password" according to the documentation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Check list for ITCareer's website registration form </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Testing of field "email" according to the documentation</t>
+  </si>
+  <si>
+    <t>Enter "Ler#1", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "Le#1", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>"Lera#1", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "Le ra1#", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "Lera1", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "Lera#", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "lera1#", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "Лера1#", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Filling the field "password" with 2 special characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Filling the field "password" with 2 numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Filling the field "password" with 2 uppercase letters</t>
+  </si>
+  <si>
+    <t>Enter "Lera1!#", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "Lera12", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <t>Enter "LLera12", another fields are filled due to specification</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                                                                  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Check list for ITCareer's website registration form</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (http://itcareer.pythonanywhere.com/) </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,6 +596,14 @@
     </font>
     <font>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -289,7 +667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -313,13 +691,33 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -640,17 +1038,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66C63F2-BBD5-44DB-8423-D64CF3E1EDBC}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.88671875" customWidth="1"/>
-    <col min="2" max="2" width="52.21875" customWidth="1"/>
-    <col min="3" max="3" width="53.88671875" customWidth="1"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="3" max="3" width="58.88671875" customWidth="1"/>
     <col min="4" max="4" width="81.44140625" customWidth="1"/>
     <col min="5" max="5" width="14.5546875" customWidth="1"/>
   </cols>
@@ -660,11 +1058,9 @@
         <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>12</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="C1" s="21"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
@@ -674,7 +1070,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -702,13 +1098,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="5"/>
     </row>
@@ -717,16 +1113,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="5"/>
     </row>
@@ -735,10 +1131,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>7</v>
@@ -753,16 +1149,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -771,10 +1167,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>7</v>
@@ -785,32 +1181,32 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+      <c r="A9" s="10">
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>7</v>
@@ -820,18 +1216,18 @@
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
+    <row r="11" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>6</v>
@@ -843,37 +1239,38 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
-        <v>10</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -881,10 +1278,10 @@
         <v>34</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>6</v>
@@ -895,16 +1292,16 @@
         <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -912,16 +1309,16 @@
         <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -929,33 +1326,33 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -963,16 +1360,16 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -980,68 +1377,88 @@
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="12" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
-        <v>18</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>19</v>
+    <row r="21" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="15">
+        <v>18</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="12" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" s="11" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>19</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>19</v>
+      <c r="B22" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="12" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10">
+    <row r="23" spans="1:5" s="11" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15">
         <v>20</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>19</v>
+      <c r="B23" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="24" spans="1:5" s="11" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>21</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1051,12 +1468,1193 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8349F83D-A97C-4C71-B9AA-BF54AD769675}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="58.5546875" customWidth="1"/>
+    <col min="3" max="3" width="59.5546875" customWidth="1"/>
+    <col min="4" max="4" width="75.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="12">
+        <v>14</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="12">
+        <v>16</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12">
+        <v>18</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="13">
+        <v>19</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="12">
+        <v>20</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="13">
+        <v>21</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A180AD-D454-4774-BAF1-205CCC327F42}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="75.88671875" customWidth="1"/>
+    <col min="3" max="3" width="79.5546875" customWidth="1"/>
+    <col min="4" max="4" width="77.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="12">
+        <v>14</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="12">
+        <v>16</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12">
+        <v>18</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="13">
+        <v>19</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="12">
+        <v>20</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="13">
+        <v>21</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12">
+        <v>22</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{208099A5-1A7C-46CD-A056-3B64820C4E7B}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="58.77734375" customWidth="1"/>
+    <col min="3" max="3" width="126.77734375" customWidth="1"/>
+    <col min="4" max="4" width="77.77734375" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="12">
+        <v>14</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="20"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="20"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="20"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="15"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>